<commit_message>
DP: create_forecast_basic - utils - monitoring_df.ipynb - percentage growth BaseProjections U_Orthodox age15_24 & percentage growth BaseProjections age20_29
</commit_message>
<xml_diff>
--- a/create_forecast_basic/utils/monitoring_df_fixed.xlsx
+++ b/create_forecast_basic/utils/monitoring_df_fixed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
   <si>
     <t>2020</t>
   </si>
@@ -220,6 +220,9 @@
     <t>percentage growth arabs_behined_seperation_wall 2045-2050</t>
   </si>
   <si>
+    <t>percentage growth BaseProjections age20_29 2020-2025</t>
+  </si>
+  <si>
     <t>percentage growth BaseProjections age20_29 2025-2030</t>
   </si>
   <si>
@@ -233,6 +236,24 @@
   </si>
   <si>
     <t>percentage growth BaseProjections age20_29 2045-2050</t>
+  </si>
+  <si>
+    <t>percentage growth BaseProjections U_Orthodox age15_24 2020-2025</t>
+  </si>
+  <si>
+    <t>percentage growth BaseProjections U_Orthodox age15_24 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth BaseProjections U_Orthodox age15_24 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth BaseProjections U_Orthodox age15_24 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth BaseProjections U_Orthodox age15_24 2040-2045</t>
+  </si>
+  <si>
+    <t>percentage growth BaseProjections U_Orthodox age15_24 2045-2050</t>
   </si>
   <si>
     <t>1,758,461</t>
@@ -644,7 +665,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -669,16 +690,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -686,16 +707,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -703,16 +724,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -720,16 +741,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -822,16 +843,16 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -839,16 +860,16 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -856,16 +877,16 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -873,16 +894,16 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -890,16 +911,16 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D15" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -907,16 +928,16 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E16" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1077,7 +1098,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C26">
         <v>288.1410644079083</v>
@@ -1094,7 +1115,7 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C27">
         <v>110.4611796870228</v>
@@ -1111,7 +1132,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C28">
         <v>109.975617699839</v>
@@ -1128,7 +1149,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C29">
         <v>109.051601597595</v>
@@ -1145,7 +1166,7 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C30">
         <v>94.67184495473032</v>
@@ -1162,7 +1183,7 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C31">
         <v>100</v>
@@ -1179,7 +1200,7 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C32">
         <v>100</v>
@@ -1196,7 +1217,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C33">
         <v>100</v>
@@ -1213,7 +1234,7 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C34">
         <v>100</v>
@@ -1230,7 +1251,7 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C35">
         <v>100</v>
@@ -1667,16 +1688,16 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C66">
-        <v>112.8455840496009</v>
+        <v>114.7293671382615</v>
       </c>
       <c r="D66">
-        <v>111.2912114030979</v>
+        <v>114.8460357932154</v>
       </c>
       <c r="E66">
-        <v>114.4679416256547</v>
+        <v>117.236732226228</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1684,16 +1705,16 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C67">
-        <v>111.0718324025138</v>
+        <v>112.8455840496009</v>
       </c>
       <c r="D67">
-        <v>111.595294236761</v>
+        <v>111.2912114030979</v>
       </c>
       <c r="E67">
-        <v>113.9493834526651</v>
+        <v>114.4679416256547</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1701,16 +1722,16 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C68">
-        <v>111.0021464070356</v>
+        <v>111.0718324025138</v>
       </c>
       <c r="D68">
-        <v>108.2587613381919</v>
+        <v>111.595294236761</v>
       </c>
       <c r="E68">
-        <v>110.9620476610768</v>
+        <v>113.9493834526651</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1718,16 +1739,16 @@
         <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C69">
-        <v>116.6204415945845</v>
+        <v>111.0021464070356</v>
       </c>
       <c r="D69">
-        <v>108.4470054591429</v>
+        <v>108.2587613381919</v>
       </c>
       <c r="E69">
-        <v>110.8047012503858</v>
+        <v>110.9620476610768</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1735,16 +1756,135 @@
         <v>72</v>
       </c>
       <c r="B70" t="s">
+        <v>81</v>
+      </c>
+      <c r="C70">
+        <v>116.6204415945845</v>
+      </c>
+      <c r="D70">
+        <v>108.4470054591429</v>
+      </c>
+      <c r="E70">
+        <v>110.8047012503858</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" t="s">
+        <v>81</v>
+      </c>
+      <c r="C71">
+        <v>106.4850397874526</v>
+      </c>
+      <c r="D71">
+        <v>108.5232023695318</v>
+      </c>
+      <c r="E71">
+        <v>111.329329828833</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C70">
-        <v>106.4850397874526</v>
-      </c>
-      <c r="D70">
-        <v>108.5232023695318</v>
-      </c>
-      <c r="E70">
-        <v>111.329329828833</v>
+      <c r="B72" t="s">
+        <v>81</v>
+      </c>
+      <c r="C72">
+        <v>142.0969095486554</v>
+      </c>
+      <c r="D72">
+        <v>140.434925384026</v>
+      </c>
+      <c r="E72">
+        <v>143.6102090706754</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" t="s">
+        <v>81</v>
+      </c>
+      <c r="C73">
+        <v>115.7775809164324</v>
+      </c>
+      <c r="D73">
+        <v>112.0281119280833</v>
+      </c>
+      <c r="E73">
+        <v>115.1755940471427</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74" t="s">
+        <v>81</v>
+      </c>
+      <c r="C74">
+        <v>114.695934706913</v>
+      </c>
+      <c r="D74">
+        <v>117.6768672379605</v>
+      </c>
+      <c r="E74">
+        <v>120.6150146970424</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75" t="s">
+        <v>81</v>
+      </c>
+      <c r="C75">
+        <v>109.3647425082543</v>
+      </c>
+      <c r="D75">
+        <v>116.9627812102758</v>
+      </c>
+      <c r="E75">
+        <v>121.2816057793425</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B76" t="s">
+        <v>81</v>
+      </c>
+      <c r="C76">
+        <v>118.4482369946029</v>
+      </c>
+      <c r="D76">
+        <v>114.1711950798264</v>
+      </c>
+      <c r="E76">
+        <v>118.1768486927674</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" t="s">
+        <v>81</v>
+      </c>
+      <c r="C77">
+        <v>106.3477491799425</v>
+      </c>
+      <c r="D77">
+        <v>112.198235626183</v>
+      </c>
+      <c r="E77">
+        <v>116.2726895715698</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DP: create_forecast_basic - utils - monitoring_df.ipynb - percentage growth student_yeshiva_and_kollim
</commit_message>
<xml_diff>
--- a/create_forecast_basic/utils/monitoring_df_fixed.xlsx
+++ b/create_forecast_basic/utils/monitoring_df_fixed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="106">
   <si>
     <t>2020</t>
   </si>
@@ -112,6 +112,9 @@
     <t>percentage growth pop 2035-2040</t>
   </si>
   <si>
+    <t>percentage growth pop 2040-2045</t>
+  </si>
+  <si>
     <t>percentage growth pop 2045-2050</t>
   </si>
   <si>
@@ -127,9 +130,30 @@
     <t>percentage growth univ 2035-2040</t>
   </si>
   <si>
+    <t>percentage growth univ 2040-2045</t>
+  </si>
+  <si>
     <t>percentage growth univ 2045-2050</t>
   </si>
   <si>
+    <t>percentage growth student_yeshiva_and_kollim 2020-2025</t>
+  </si>
+  <si>
+    <t>percentage growth student_yeshiva_and_kollim 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth student_yeshiva_and_kollim 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth student_yeshiva_and_kollim 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth student_yeshiva_and_kollim 2040-2045</t>
+  </si>
+  <si>
+    <t>percentage growth student_yeshiva_and_kollim 2045-2050</t>
+  </si>
+  <si>
     <t>percentage growth Arab 2020-2025</t>
   </si>
   <si>
@@ -220,40 +244,40 @@
     <t>percentage growth arabs_behined_seperation_wall 2045-2050</t>
   </si>
   <si>
-    <t>percentage growth BaseProjections age20_29 2020-2025</t>
-  </si>
-  <si>
-    <t>percentage growth BaseProjections age20_29 2025-2030</t>
-  </si>
-  <si>
-    <t>percentage growth BaseProjections age20_29 2030-2035</t>
-  </si>
-  <si>
-    <t>percentage growth BaseProjections age20_29 2035-2040</t>
-  </si>
-  <si>
-    <t>percentage growth BaseProjections age20_29 2040-2045</t>
-  </si>
-  <si>
-    <t>percentage growth BaseProjections age20_29 2045-2050</t>
-  </si>
-  <si>
-    <t>percentage growth BaseProjections U_Orthodox age15_24 2020-2025</t>
-  </si>
-  <si>
-    <t>percentage growth BaseProjections U_Orthodox age15_24 2025-2030</t>
-  </si>
-  <si>
-    <t>percentage growth BaseProjections U_Orthodox age15_24 2030-2035</t>
-  </si>
-  <si>
-    <t>percentage growth BaseProjections U_Orthodox age15_24 2035-2040</t>
-  </si>
-  <si>
-    <t>percentage growth BaseProjections U_Orthodox age15_24 2040-2045</t>
-  </si>
-  <si>
-    <t>percentage growth BaseProjections U_Orthodox age15_24 2045-2050</t>
+    <t>percentage growth age20_29 2020-2025</t>
+  </si>
+  <si>
+    <t>percentage growth age20_29 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth age20_29 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth age20_29 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth age20_29 2040-2045</t>
+  </si>
+  <si>
+    <t>percentage growth age20_29 2045-2050</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox age15_24 2020-2025</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox age15_24 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox age15_24 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox age15_24 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox age15_24 2040-2045</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox age15_24 2045-2050</t>
   </si>
   <si>
     <t>1,758,461</t>
@@ -665,7 +689,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -690,16 +714,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -707,16 +731,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -724,16 +748,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -741,16 +765,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -843,16 +867,16 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="E11" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -860,16 +884,16 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="E12" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -877,16 +901,16 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -894,16 +918,16 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E14" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -911,16 +935,16 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D15" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -928,16 +952,16 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="D16" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="E16" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1098,7 +1122,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C26">
         <v>288.1410644079083</v>
@@ -1115,7 +1139,7 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C27">
         <v>110.4611796870228</v>
@@ -1132,7 +1156,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C28">
         <v>109.975617699839</v>
@@ -1149,7 +1173,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C29">
         <v>109.051601597595</v>
@@ -1166,16 +1190,16 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C30">
-        <v>94.67184495473032</v>
+        <v>106.5666906077168</v>
       </c>
       <c r="D30">
-        <v>93.61444029023103</v>
+        <v>106.8272018621244</v>
       </c>
       <c r="E30">
-        <v>92.48650039603555</v>
+        <v>108.1656551990757</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1183,16 +1207,16 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C31">
-        <v>100</v>
+        <v>105.6280249400627</v>
       </c>
       <c r="D31">
-        <v>100</v>
+        <v>106.8211268368127</v>
       </c>
       <c r="E31">
-        <v>100</v>
+        <v>108.1238878882766</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1200,7 +1224,7 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C32">
         <v>100</v>
@@ -1217,7 +1241,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C33">
         <v>100</v>
@@ -1234,7 +1258,7 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C34">
         <v>100</v>
@@ -1251,7 +1275,7 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C35">
         <v>100</v>
@@ -1267,112 +1291,136 @@
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
       <c r="C36">
-        <v>112.3202972412109</v>
+        <v>100</v>
       </c>
       <c r="D36">
-        <v>111.3030700683594</v>
+        <v>100</v>
       </c>
       <c r="E36">
-        <v>111.842399597168</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="B37" t="s">
+        <v>89</v>
+      </c>
       <c r="C37">
-        <v>114.3151168823242</v>
+        <v>100</v>
       </c>
       <c r="D37">
-        <v>107.5494537353516</v>
+        <v>100</v>
       </c>
       <c r="E37">
-        <v>109.3707275390625</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
       <c r="C38">
-        <v>0</v>
+        <v>141.7442130435599</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>140.1409664231686</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>143.461271155046</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="B39" t="s">
+        <v>89</v>
+      </c>
       <c r="C39">
-        <v>122.9322967529297</v>
+        <v>117.9048074979183</v>
       </c>
       <c r="D39">
-        <v>120.7884521484375</v>
+        <v>114.6623810975685</v>
       </c>
       <c r="E39">
-        <v>123.14892578125</v>
+        <v>118.4549776699289</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="B40" t="s">
+        <v>89</v>
+      </c>
       <c r="C40">
-        <v>114.5723495483398</v>
+        <v>116.3179437560024</v>
       </c>
       <c r="D40">
-        <v>113.2040252685547</v>
+        <v>119.126401924712</v>
       </c>
       <c r="E40">
-        <v>113.7573547363281</v>
+        <v>122.4437430459023</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="B41" t="s">
+        <v>89</v>
+      </c>
       <c r="C41">
-        <v>111.661750793457</v>
+        <v>109.9752461808908</v>
       </c>
       <c r="D41">
-        <v>108.5102615356445</v>
+        <v>118.3491128670014</v>
       </c>
       <c r="E41">
-        <v>109.7856826782227</v>
+        <v>123.2056920173415</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
       <c r="C42">
-        <v>114.0274200439453</v>
+        <v>118.1238187244034</v>
       </c>
       <c r="D42">
-        <v>108.323356628418</v>
+        <v>115.2764931719222</v>
       </c>
       <c r="E42">
-        <v>111.0597229003906</v>
+        <v>119.3997172692221</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="B43" t="s">
+        <v>89</v>
+      </c>
       <c r="C43">
-        <v>108.2132720947266</v>
+        <v>106.6086767449847</v>
       </c>
       <c r="D43">
-        <v>108.2132720947266</v>
+        <v>113.4838191485299</v>
       </c>
       <c r="E43">
-        <v>108.2132720947266</v>
+        <v>117.6148091351713</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1380,13 +1428,13 @@
         <v>46</v>
       </c>
       <c r="C44">
-        <v>114.3493194580078</v>
+        <v>112.3202972412109</v>
       </c>
       <c r="D44">
-        <v>116.0060729980469</v>
+        <v>111.3030700683594</v>
       </c>
       <c r="E44">
-        <v>119.6857528686523</v>
+        <v>111.842399597168</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1394,13 +1442,13 @@
         <v>47</v>
       </c>
       <c r="C45">
-        <v>113.9139022827148</v>
+        <v>114.3151168823242</v>
       </c>
       <c r="D45">
-        <v>110.5818710327148</v>
+        <v>107.5494537353516</v>
       </c>
       <c r="E45">
-        <v>111.8965606689453</v>
+        <v>109.3707275390625</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1408,13 +1456,13 @@
         <v>48</v>
       </c>
       <c r="C46">
-        <v>111.4065017700195</v>
+        <v>0</v>
       </c>
       <c r="D46">
-        <v>108.8073043823242</v>
+        <v>0</v>
       </c>
       <c r="E46">
-        <v>110.0499496459961</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1422,13 +1470,13 @@
         <v>49</v>
       </c>
       <c r="C47">
-        <v>115.2005615234375</v>
+        <v>122.9322967529297</v>
       </c>
       <c r="D47">
-        <v>108.5818710327148</v>
+        <v>120.7884521484375</v>
       </c>
       <c r="E47">
-        <v>110.9671173095703</v>
+        <v>123.14892578125</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1436,13 +1484,13 @@
         <v>50</v>
       </c>
       <c r="C48">
-        <v>107.2044982910156</v>
+        <v>114.5723495483398</v>
       </c>
       <c r="D48">
-        <v>107.2044982910156</v>
+        <v>113.2040252685547</v>
       </c>
       <c r="E48">
-        <v>107.2044982910156</v>
+        <v>113.7573547363281</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1450,13 +1498,13 @@
         <v>51</v>
       </c>
       <c r="C49">
-        <v>113.8025817871094</v>
+        <v>111.661750793457</v>
       </c>
       <c r="D49">
-        <v>115.0981063842773</v>
+        <v>108.5102615356445</v>
       </c>
       <c r="E49">
-        <v>118.8546524047852</v>
+        <v>109.7856826782227</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1464,13 +1512,13 @@
         <v>52</v>
       </c>
       <c r="C50">
-        <v>109.2754135131836</v>
+        <v>114.0274200439453</v>
       </c>
       <c r="D50">
-        <v>106.5745468139648</v>
+        <v>108.323356628418</v>
       </c>
       <c r="E50">
-        <v>107.8064422607422</v>
+        <v>111.0597229003906</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1478,13 +1526,13 @@
         <v>53</v>
       </c>
       <c r="C51">
-        <v>111.4402313232422</v>
+        <v>108.2132720947266</v>
       </c>
       <c r="D51">
-        <v>108.4855270385742</v>
+        <v>108.2132720947266</v>
       </c>
       <c r="E51">
-        <v>110.432861328125</v>
+        <v>108.2132720947266</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1492,13 +1540,13 @@
         <v>54</v>
       </c>
       <c r="C52">
-        <v>115.7983703613281</v>
+        <v>114.3493194580078</v>
       </c>
       <c r="D52">
-        <v>107.3515243530273</v>
+        <v>116.0060729980469</v>
       </c>
       <c r="E52">
-        <v>109.9095687866211</v>
+        <v>119.6857528686523</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1506,13 +1554,13 @@
         <v>55</v>
       </c>
       <c r="C53">
-        <v>106.3913955688477</v>
+        <v>113.9139022827148</v>
       </c>
       <c r="D53">
-        <v>106.3913955688477</v>
+        <v>110.5818710327148</v>
       </c>
       <c r="E53">
-        <v>106.3913955688477</v>
+        <v>111.8965606689453</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1520,13 +1568,13 @@
         <v>56</v>
       </c>
       <c r="C54">
-        <v>109.6991577148438</v>
+        <v>111.4065017700195</v>
       </c>
       <c r="D54">
-        <v>113.7160949707031</v>
+        <v>108.8073043823242</v>
       </c>
       <c r="E54">
-        <v>118.3788070678711</v>
+        <v>110.0499496459961</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1534,13 +1582,13 @@
         <v>57</v>
       </c>
       <c r="C55">
-        <v>103.6191787719727</v>
+        <v>115.2005615234375</v>
       </c>
       <c r="D55">
-        <v>100.9641647338867</v>
+        <v>108.5818710327148</v>
       </c>
       <c r="E55">
-        <v>102.7881393432617</v>
+        <v>110.9671173095703</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1548,13 +1596,13 @@
         <v>58</v>
       </c>
       <c r="C56">
-        <v>108.0526351928711</v>
+        <v>107.2044982910156</v>
       </c>
       <c r="D56">
-        <v>107.7009811401367</v>
+        <v>107.2044982910156</v>
       </c>
       <c r="E56">
-        <v>109.5689926147461</v>
+        <v>107.2044982910156</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1562,13 +1610,13 @@
         <v>59</v>
       </c>
       <c r="C57">
-        <v>108.9937896728516</v>
+        <v>113.8025817871094</v>
       </c>
       <c r="D57">
-        <v>104.2914199829102</v>
+        <v>115.0981063842773</v>
       </c>
       <c r="E57">
-        <v>106.7485198974609</v>
+        <v>118.8546524047852</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1576,13 +1624,13 @@
         <v>60</v>
       </c>
       <c r="C58">
-        <v>105.8768997192383</v>
+        <v>109.2754135131836</v>
       </c>
       <c r="D58">
-        <v>105.8768997192383</v>
+        <v>106.5745468139648</v>
       </c>
       <c r="E58">
-        <v>105.8768997192383</v>
+        <v>107.8064422607422</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1590,13 +1638,13 @@
         <v>61</v>
       </c>
       <c r="C59">
-        <v>105.8174667358398</v>
+        <v>111.4402313232422</v>
       </c>
       <c r="D59">
-        <v>114.2177886962891</v>
+        <v>108.4855270385742</v>
       </c>
       <c r="E59">
-        <v>117.9976348876953</v>
+        <v>110.432861328125</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1604,13 +1652,13 @@
         <v>62</v>
       </c>
       <c r="C60">
-        <v>100.2247543334961</v>
+        <v>115.7983703613281</v>
       </c>
       <c r="D60">
-        <v>99.93392944335938</v>
+        <v>107.3515243530273</v>
       </c>
       <c r="E60">
-        <v>101.6650161743164</v>
+        <v>109.9095687866211</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1618,13 +1666,13 @@
         <v>63</v>
       </c>
       <c r="C61">
-        <v>100.3374252319336</v>
+        <v>106.3913955688477</v>
       </c>
       <c r="D61">
-        <v>105.1654663085938</v>
+        <v>106.3913955688477</v>
       </c>
       <c r="E61">
-        <v>106.7888488769531</v>
+        <v>106.3913955688477</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1632,13 +1680,13 @@
         <v>64</v>
       </c>
       <c r="C62">
-        <v>107.3705596923828</v>
+        <v>109.6991577148438</v>
       </c>
       <c r="D62">
-        <v>103.8991165161133</v>
+        <v>113.7160949707031</v>
       </c>
       <c r="E62">
-        <v>106.160888671875</v>
+        <v>118.3788070678711</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1646,13 +1694,13 @@
         <v>65</v>
       </c>
       <c r="C63">
-        <v>105.9054794311523</v>
+        <v>103.6191787719727</v>
       </c>
       <c r="D63">
-        <v>105.9054794311523</v>
+        <v>100.9641647338867</v>
       </c>
       <c r="E63">
-        <v>105.9054794311523</v>
+        <v>102.7881393432617</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1660,13 +1708,13 @@
         <v>66</v>
       </c>
       <c r="C64">
-        <v>104.9963073730469</v>
+        <v>108.0526351928711</v>
       </c>
       <c r="D64">
-        <v>114.1932830810547</v>
+        <v>107.7009811401367</v>
       </c>
       <c r="E64">
-        <v>117.6402359008789</v>
+        <v>109.5689926147461</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1674,149 +1722,125 @@
         <v>67</v>
       </c>
       <c r="C65">
-        <v>100</v>
+        <v>108.9937896728516</v>
       </c>
       <c r="D65">
-        <v>104.9321594238281</v>
+        <v>104.2914199829102</v>
       </c>
       <c r="E65">
-        <v>106.5721893310547</v>
+        <v>106.7485198974609</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B66" t="s">
-        <v>81</v>
-      </c>
       <c r="C66">
-        <v>114.7293671382615</v>
+        <v>105.8768997192383</v>
       </c>
       <c r="D66">
-        <v>114.8460357932154</v>
+        <v>105.8768997192383</v>
       </c>
       <c r="E66">
-        <v>117.236732226228</v>
+        <v>105.8768997192383</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B67" t="s">
-        <v>81</v>
-      </c>
       <c r="C67">
-        <v>112.8455840496009</v>
+        <v>105.8174667358398</v>
       </c>
       <c r="D67">
-        <v>111.2912114030979</v>
+        <v>114.2177886962891</v>
       </c>
       <c r="E67">
-        <v>114.4679416256547</v>
+        <v>117.9976348876953</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B68" t="s">
-        <v>81</v>
-      </c>
       <c r="C68">
-        <v>111.0718324025138</v>
+        <v>100.2247543334961</v>
       </c>
       <c r="D68">
-        <v>111.595294236761</v>
+        <v>99.93392944335938</v>
       </c>
       <c r="E68">
-        <v>113.9493834526651</v>
+        <v>101.6650161743164</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B69" t="s">
-        <v>81</v>
-      </c>
       <c r="C69">
-        <v>111.0021464070356</v>
+        <v>100.3374252319336</v>
       </c>
       <c r="D69">
-        <v>108.2587613381919</v>
+        <v>105.1654663085938</v>
       </c>
       <c r="E69">
-        <v>110.9620476610768</v>
+        <v>106.7888488769531</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B70" t="s">
-        <v>81</v>
-      </c>
       <c r="C70">
-        <v>116.6204415945845</v>
+        <v>107.3705596923828</v>
       </c>
       <c r="D70">
-        <v>108.4470054591429</v>
+        <v>103.8991165161133</v>
       </c>
       <c r="E70">
-        <v>110.8047012503858</v>
+        <v>106.160888671875</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B71" t="s">
-        <v>81</v>
-      </c>
       <c r="C71">
-        <v>106.4850397874526</v>
+        <v>105.9054794311523</v>
       </c>
       <c r="D71">
-        <v>108.5232023695318</v>
+        <v>105.9054794311523</v>
       </c>
       <c r="E71">
-        <v>111.329329828833</v>
+        <v>105.9054794311523</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B72" t="s">
-        <v>81</v>
-      </c>
       <c r="C72">
-        <v>142.0969095486554</v>
+        <v>104.9963073730469</v>
       </c>
       <c r="D72">
-        <v>140.434925384026</v>
+        <v>114.1932830810547</v>
       </c>
       <c r="E72">
-        <v>143.6102090706754</v>
+        <v>117.6402359008789</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B73" t="s">
-        <v>81</v>
-      </c>
       <c r="C73">
-        <v>115.7775809164324</v>
+        <v>100</v>
       </c>
       <c r="D73">
-        <v>112.0281119280833</v>
+        <v>104.9321594238281</v>
       </c>
       <c r="E73">
-        <v>115.1755940471427</v>
+        <v>106.5721893310547</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -1824,16 +1848,16 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C74">
-        <v>114.695934706913</v>
+        <v>114.7293671382615</v>
       </c>
       <c r="D74">
-        <v>117.6768672379605</v>
+        <v>114.8460357932154</v>
       </c>
       <c r="E74">
-        <v>120.6150146970424</v>
+        <v>117.236732226228</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1841,16 +1865,16 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C75">
-        <v>109.3647425082543</v>
+        <v>112.8455840496009</v>
       </c>
       <c r="D75">
-        <v>116.9627812102758</v>
+        <v>111.2912114030979</v>
       </c>
       <c r="E75">
-        <v>121.2816057793425</v>
+        <v>114.4679416256547</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1858,16 +1882,16 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C76">
-        <v>118.4482369946029</v>
+        <v>111.0718324025138</v>
       </c>
       <c r="D76">
-        <v>114.1711950798264</v>
+        <v>111.595294236761</v>
       </c>
       <c r="E76">
-        <v>118.1768486927674</v>
+        <v>113.9493834526651</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1875,15 +1899,151 @@
         <v>79</v>
       </c>
       <c r="B77" t="s">
+        <v>89</v>
+      </c>
+      <c r="C77">
+        <v>111.0021464070356</v>
+      </c>
+      <c r="D77">
+        <v>108.2587613381919</v>
+      </c>
+      <c r="E77">
+        <v>110.9620476610768</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B78" t="s">
+        <v>89</v>
+      </c>
+      <c r="C78">
+        <v>116.6204415945845</v>
+      </c>
+      <c r="D78">
+        <v>108.4470054591429</v>
+      </c>
+      <c r="E78">
+        <v>110.8047012503858</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C77">
+      <c r="B79" t="s">
+        <v>89</v>
+      </c>
+      <c r="C79">
+        <v>106.4850397874526</v>
+      </c>
+      <c r="D79">
+        <v>108.5232023695318</v>
+      </c>
+      <c r="E79">
+        <v>111.329329828833</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B80" t="s">
+        <v>89</v>
+      </c>
+      <c r="C80">
+        <v>142.0969095486554</v>
+      </c>
+      <c r="D80">
+        <v>140.434925384026</v>
+      </c>
+      <c r="E80">
+        <v>143.6102090706754</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B81" t="s">
+        <v>89</v>
+      </c>
+      <c r="C81">
+        <v>115.7775809164324</v>
+      </c>
+      <c r="D81">
+        <v>112.0281119280833</v>
+      </c>
+      <c r="E81">
+        <v>115.1755940471427</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B82" t="s">
+        <v>89</v>
+      </c>
+      <c r="C82">
+        <v>114.695934706913</v>
+      </c>
+      <c r="D82">
+        <v>117.6768672379605</v>
+      </c>
+      <c r="E82">
+        <v>120.6150146970424</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B83" t="s">
+        <v>89</v>
+      </c>
+      <c r="C83">
+        <v>109.3647425082543</v>
+      </c>
+      <c r="D83">
+        <v>116.9627812102758</v>
+      </c>
+      <c r="E83">
+        <v>121.2816057793425</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B84" t="s">
+        <v>89</v>
+      </c>
+      <c r="C84">
+        <v>118.4482369946029</v>
+      </c>
+      <c r="D84">
+        <v>114.1711950798264</v>
+      </c>
+      <c r="E84">
+        <v>118.1768486927674</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B85" t="s">
+        <v>89</v>
+      </c>
+      <c r="C85">
         <v>106.3477491799425</v>
       </c>
-      <c r="D77">
+      <c r="D85">
         <v>112.198235626183</v>
       </c>
-      <c r="E77">
+      <c r="E85">
         <v>116.2726895715698</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DP: create_forecast_basic - utils - monitoring_df.ipynb - percentage growth age20_29 per sector
</commit_message>
<xml_diff>
--- a/create_forecast_basic/utils/monitoring_df_fixed.xlsx
+++ b/create_forecast_basic/utils/monitoring_df_fixed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="130">
   <si>
     <t>2020</t>
   </si>
@@ -244,24 +244,6 @@
     <t>percentage growth arabs_behined_seperation_wall 2045-2050</t>
   </si>
   <si>
-    <t>percentage growth age20_29 2020-2025</t>
-  </si>
-  <si>
-    <t>percentage growth age20_29 2025-2030</t>
-  </si>
-  <si>
-    <t>percentage growth age20_29 2030-2035</t>
-  </si>
-  <si>
-    <t>percentage growth age20_29 2035-2040</t>
-  </si>
-  <si>
-    <t>percentage growth age20_29 2040-2045</t>
-  </si>
-  <si>
-    <t>percentage growth age20_29 2045-2050</t>
-  </si>
-  <si>
     <t>percentage growth U_Orthodox age15_24 2020-2025</t>
   </si>
   <si>
@@ -278,6 +260,96 @@
   </si>
   <si>
     <t>percentage growth U_Orthodox age15_24 2045-2050</t>
+  </si>
+  <si>
+    <t>percentage growth Arab age20_29 2020-2025</t>
+  </si>
+  <si>
+    <t>percentage growth Arab age20_29 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth Arab age20_29 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth Arab age20_29 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth Arab age20_29 2040-2045</t>
+  </si>
+  <si>
+    <t>percentage growth Arab age20_29 2045-2050</t>
+  </si>
+  <si>
+    <t>percentage growth Jewish age20_29 2020-2025</t>
+  </si>
+  <si>
+    <t>percentage growth Jewish age20_29 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth Jewish age20_29 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth Jewish age20_29 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth Jewish age20_29 2040-2045</t>
+  </si>
+  <si>
+    <t>percentage growth Jewish age20_29 2045-2050</t>
+  </si>
+  <si>
+    <t>percentage growth Palestinian age20_29 2020-2025</t>
+  </si>
+  <si>
+    <t>percentage growth Palestinian age20_29 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth Palestinian age20_29 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth Palestinian age20_29 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth Palestinian age20_29 2040-2045</t>
+  </si>
+  <si>
+    <t>percentage growth Palestinian age20_29 2045-2050</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox age20_29 2020-2025</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox age20_29 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox age20_29 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox age20_29 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox age20_29 2040-2045</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox age20_29 2045-2050</t>
+  </si>
+  <si>
+    <t>percentage growth arabs_behined_seperation_wall age20_29 2020-2025</t>
+  </si>
+  <si>
+    <t>percentage growth arabs_behined_seperation_wall age20_29 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth arabs_behined_seperation_wall age20_29 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth arabs_behined_seperation_wall age20_29 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth arabs_behined_seperation_wall age20_29 2040-2045</t>
+  </si>
+  <si>
+    <t>percentage growth arabs_behined_seperation_wall age20_29 2045-2050</t>
   </si>
   <si>
     <t>1,758,461</t>
@@ -689,7 +761,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -714,16 +786,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -731,16 +803,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -748,16 +820,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -765,16 +837,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -867,16 +939,16 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="E11" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -884,16 +956,16 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="E12" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -901,16 +973,16 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="E13" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -918,16 +990,16 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="D14" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="E14" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -935,16 +1007,16 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -952,16 +1024,16 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C16" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="D16" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="E16" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1122,7 +1194,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C26">
         <v>288.1410644079083</v>
@@ -1139,7 +1211,7 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C27">
         <v>110.4611796870228</v>
@@ -1156,7 +1228,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C28">
         <v>109.975617699839</v>
@@ -1173,7 +1245,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C29">
         <v>109.051601597595</v>
@@ -1190,7 +1262,7 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C30">
         <v>106.5666906077168</v>
@@ -1207,7 +1279,7 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C31">
         <v>105.6280249400627</v>
@@ -1224,7 +1296,7 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C32">
         <v>100</v>
@@ -1241,7 +1313,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C33">
         <v>100</v>
@@ -1258,7 +1330,7 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C34">
         <v>100</v>
@@ -1275,7 +1347,7 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C35">
         <v>100</v>
@@ -1292,7 +1364,7 @@
         <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C36">
         <v>100</v>
@@ -1309,7 +1381,7 @@
         <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C37">
         <v>100</v>
@@ -1326,7 +1398,7 @@
         <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C38">
         <v>141.7442130435599</v>
@@ -1343,7 +1415,7 @@
         <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C39">
         <v>117.9048074979183</v>
@@ -1360,7 +1432,7 @@
         <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C40">
         <v>116.3179437560024</v>
@@ -1377,7 +1449,7 @@
         <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C41">
         <v>109.9752461808908</v>
@@ -1394,7 +1466,7 @@
         <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C42">
         <v>118.1238187244034</v>
@@ -1411,7 +1483,7 @@
         <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C43">
         <v>106.6086767449847</v>
@@ -1848,16 +1920,16 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C74">
-        <v>114.7293671382615</v>
+        <v>142.0969095486554</v>
       </c>
       <c r="D74">
-        <v>114.8460357932154</v>
+        <v>140.434925384026</v>
       </c>
       <c r="E74">
-        <v>117.236732226228</v>
+        <v>143.6102090706754</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1865,16 +1937,16 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C75">
-        <v>112.8455840496009</v>
+        <v>115.7775809164324</v>
       </c>
       <c r="D75">
-        <v>111.2912114030979</v>
+        <v>112.0281119280833</v>
       </c>
       <c r="E75">
-        <v>114.4679416256547</v>
+        <v>115.1755940471427</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1882,16 +1954,16 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C76">
-        <v>111.0718324025138</v>
+        <v>114.695934706913</v>
       </c>
       <c r="D76">
-        <v>111.595294236761</v>
+        <v>117.6768672379605</v>
       </c>
       <c r="E76">
-        <v>113.9493834526651</v>
+        <v>120.6150146970424</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1899,16 +1971,16 @@
         <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C77">
-        <v>111.0021464070356</v>
+        <v>109.3647425082543</v>
       </c>
       <c r="D77">
-        <v>108.2587613381919</v>
+        <v>116.9627812102758</v>
       </c>
       <c r="E77">
-        <v>110.9620476610768</v>
+        <v>121.2816057793425</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -1916,16 +1988,16 @@
         <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C78">
-        <v>116.6204415945845</v>
+        <v>118.4482369946029</v>
       </c>
       <c r="D78">
-        <v>108.4470054591429</v>
+        <v>114.1711950798264</v>
       </c>
       <c r="E78">
-        <v>110.8047012503858</v>
+        <v>118.1768486927674</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -1933,16 +2005,16 @@
         <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C79">
-        <v>106.4850397874526</v>
+        <v>106.3477491799425</v>
       </c>
       <c r="D79">
-        <v>108.5232023695318</v>
+        <v>112.198235626183</v>
       </c>
       <c r="E79">
-        <v>111.329329828833</v>
+        <v>116.2726895715698</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -1950,16 +2022,16 @@
         <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C80">
-        <v>142.0969095486554</v>
+        <v>113.4294983956014</v>
       </c>
       <c r="D80">
-        <v>140.434925384026</v>
+        <v>115.4259515180992</v>
       </c>
       <c r="E80">
-        <v>143.6102090706754</v>
+        <v>116.0967740022183</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -1967,16 +2039,16 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C81">
-        <v>115.7775809164324</v>
+        <v>106.0431602010029</v>
       </c>
       <c r="D81">
-        <v>112.0281119280833</v>
+        <v>101.8329248177095</v>
       </c>
       <c r="E81">
-        <v>115.1755940471427</v>
+        <v>103.2150119036671</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -1984,16 +2056,16 @@
         <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C82">
-        <v>114.695934706913</v>
+        <v>101.1114508032624</v>
       </c>
       <c r="D82">
-        <v>117.6768672379605</v>
+        <v>100.296204345676</v>
       </c>
       <c r="E82">
-        <v>120.6150146970424</v>
+        <v>101.5641163979785</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -2001,16 +2073,16 @@
         <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C83">
-        <v>109.3647425082543</v>
+        <v>110.0637886975012</v>
       </c>
       <c r="D83">
-        <v>116.9627812102758</v>
+        <v>106.0781541650525</v>
       </c>
       <c r="E83">
-        <v>121.2816057793425</v>
+        <v>108.1221885950163</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -2018,16 +2090,16 @@
         <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C84">
-        <v>118.4482369946029</v>
+        <v>111.0307149693382</v>
       </c>
       <c r="D84">
-        <v>114.1711950798264</v>
+        <v>106.014930611548</v>
       </c>
       <c r="E84">
-        <v>118.1768486927674</v>
+        <v>107.8685820145409</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2035,16 +2107,424 @@
         <v>87</v>
       </c>
       <c r="B85" t="s">
+        <v>113</v>
+      </c>
+      <c r="C85">
+        <v>102.8545432052454</v>
+      </c>
+      <c r="D85">
+        <v>104.6840607719977</v>
+      </c>
+      <c r="E85">
+        <v>106.3092840368721</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B86" t="s">
+        <v>113</v>
+      </c>
+      <c r="C86">
+        <v>106.3806513824993</v>
+      </c>
+      <c r="D86">
+        <v>103.8284757887404</v>
+      </c>
+      <c r="E86">
+        <v>106.395944045844</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C85">
-        <v>106.3477491799425</v>
-      </c>
-      <c r="D85">
-        <v>112.198235626183</v>
-      </c>
-      <c r="E85">
-        <v>116.2726895715698</v>
+      <c r="B87" t="s">
+        <v>113</v>
+      </c>
+      <c r="C87">
+        <v>112.7741561929101</v>
+      </c>
+      <c r="D87">
+        <v>112.0618444927675</v>
+      </c>
+      <c r="E87">
+        <v>115.2597085004402</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B88" t="s">
+        <v>113</v>
+      </c>
+      <c r="C88">
+        <v>113.4019669460993</v>
+      </c>
+      <c r="D88">
+        <v>116.8535346712863</v>
+      </c>
+      <c r="E88">
+        <v>118.9172571345435</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B89" t="s">
+        <v>113</v>
+      </c>
+      <c r="C89">
+        <v>114.3734758810617</v>
+      </c>
+      <c r="D89">
+        <v>104.3268044103817</v>
+      </c>
+      <c r="E89">
+        <v>106.117051103353</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B90" t="s">
+        <v>113</v>
+      </c>
+      <c r="C90">
+        <v>116.6600919190665</v>
+      </c>
+      <c r="D90">
+        <v>102.1215202231729</v>
+      </c>
+      <c r="E90">
+        <v>103.718287976195</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B91" t="s">
+        <v>113</v>
+      </c>
+      <c r="C91">
+        <v>107.8550008014949</v>
+      </c>
+      <c r="D91">
+        <v>104.3352478258511</v>
+      </c>
+      <c r="E91">
+        <v>106.5730290242286</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B92" t="s">
+        <v>113</v>
+      </c>
+      <c r="C92">
+        <v>141.2462908011869</v>
+      </c>
+      <c r="D92">
+        <v>139.4658753709199</v>
+      </c>
+      <c r="E92">
+        <v>142.1364985163205</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B93" t="s">
+        <v>113</v>
+      </c>
+      <c r="C93">
+        <v>115.9663865546219</v>
+      </c>
+      <c r="D93">
+        <v>112.3404255319149</v>
+      </c>
+      <c r="E93">
+        <v>115.2400835073069</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B94" t="s">
+        <v>113</v>
+      </c>
+      <c r="C94">
+        <v>114.3115942028985</v>
+      </c>
+      <c r="D94">
+        <v>117.8030303030303</v>
+      </c>
+      <c r="E94">
+        <v>120.8333333333333</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B95" t="s">
+        <v>113</v>
+      </c>
+      <c r="C95">
+        <v>109.6671949286846</v>
+      </c>
+      <c r="D95">
+        <v>116.5594855305467</v>
+      </c>
+      <c r="E95">
+        <v>121.4392803598201</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B96" t="s">
+        <v>113</v>
+      </c>
+      <c r="C96">
+        <v>118.3526011560694</v>
+      </c>
+      <c r="D96">
+        <v>114.2068965517241</v>
+      </c>
+      <c r="E96">
+        <v>118.3950617283951</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B97" t="s">
+        <v>113</v>
+      </c>
+      <c r="C97">
+        <v>106.7155067155067</v>
+      </c>
+      <c r="D97">
+        <v>112.56038647343</v>
+      </c>
+      <c r="E97">
+        <v>116.162669447341</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B98" t="s">
+        <v>113</v>
+      </c>
+      <c r="C98">
+        <v>127.33147663382</v>
+      </c>
+      <c r="D98">
+        <v>130.2807008982568</v>
+      </c>
+      <c r="E98">
+        <v>133.7545182980177</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B99" t="s">
+        <v>113</v>
+      </c>
+      <c r="C99">
+        <v>116.1886120996441</v>
+      </c>
+      <c r="D99">
+        <v>115.5187405855613</v>
+      </c>
+      <c r="E99">
+        <v>119.8312863051076</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B100" t="s">
+        <v>113</v>
+      </c>
+      <c r="C100">
+        <v>114.8139771037869</v>
+      </c>
+      <c r="D100">
+        <v>112.3810692878517</v>
+      </c>
+      <c r="E100">
+        <v>115.5289512314468</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B101" t="s">
+        <v>113</v>
+      </c>
+      <c r="C101">
+        <v>109.1212424047789</v>
+      </c>
+      <c r="D101">
+        <v>116.5549306398528</v>
+      </c>
+      <c r="E101">
+        <v>120.5503820371929</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B102" t="s">
+        <v>113</v>
+      </c>
+      <c r="C102">
+        <v>121.5786385638688</v>
+      </c>
+      <c r="D102">
+        <v>118.6196067891554</v>
+      </c>
+      <c r="E102">
+        <v>121.6434702631632</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B103" t="s">
+        <v>113</v>
+      </c>
+      <c r="C103">
+        <v>106.8000600146324</v>
+      </c>
+      <c r="D103">
+        <v>114.7075659012718</v>
+      </c>
+      <c r="E103">
+        <v>118.2125683242491</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B104" t="s">
+        <v>113</v>
+      </c>
+      <c r="C104">
+        <v>123.1392129562949</v>
+      </c>
+      <c r="D104">
+        <v>125.2980619968953</v>
+      </c>
+      <c r="E104">
+        <v>126.0230127866596</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B105" t="s">
+        <v>113</v>
+      </c>
+      <c r="C105">
+        <v>114.3269305746887</v>
+      </c>
+      <c r="D105">
+        <v>109.8013921706367</v>
+      </c>
+      <c r="E105">
+        <v>111.2625082541779</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B106" t="s">
+        <v>113</v>
+      </c>
+      <c r="C106">
+        <v>100.9969307718541</v>
+      </c>
+      <c r="D106">
+        <v>100.151217299259</v>
+      </c>
+      <c r="E106">
+        <v>101.4380770854971</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B107" t="s">
+        <v>113</v>
+      </c>
+      <c r="C107">
+        <v>99.18849257712696</v>
+      </c>
+      <c r="D107">
+        <v>95.7119130303488</v>
+      </c>
+      <c r="E107">
+        <v>97.55729828864612</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B108" t="s">
+        <v>113</v>
+      </c>
+      <c r="C108">
+        <v>100.6740349045685</v>
+      </c>
+      <c r="D108">
+        <v>96.06708167995436</v>
+      </c>
+      <c r="E108">
+        <v>97.73948746338201</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B109" t="s">
+        <v>113</v>
+      </c>
+      <c r="C109">
+        <v>101.2443642921551</v>
+      </c>
+      <c r="D109">
+        <v>102.992446252179</v>
+      </c>
+      <c r="E109">
+        <v>104.590187147476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DP: create_forecast_basic - utils - monitoring_df.ipynb - emp_okev at {SCHN_NAME} in {year}
</commit_message>
<xml_diff>
--- a/create_forecast_basic/utils/monitoring_df_fixed.xlsx
+++ b/create_forecast_basic/utils/monitoring_df_fixed.xlsx
@@ -2576,13 +2576,13 @@
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2">
-        <v>288.1410644079083</v>
+        <v>188.1410644079084</v>
       </c>
       <c r="D26" s="2">
-        <v>283.9696620191286</v>
+        <v>183.9696620191286</v>
       </c>
       <c r="E26" s="2">
-        <v>285.6774324006337</v>
+        <v>185.6774324006336</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -2591,13 +2591,13 @@
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2">
-        <v>110.4611796870228</v>
+        <v>10.46117968702283</v>
       </c>
       <c r="D27" s="2">
-        <v>109.2979336473809</v>
+        <v>9.297933647380905</v>
       </c>
       <c r="E27" s="2">
-        <v>110.4035195766238</v>
+        <v>10.40351957662375</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -2606,13 +2606,13 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2">
-        <v>109.975617699839</v>
+        <v>9.975617699839043</v>
       </c>
       <c r="D28" s="2">
-        <v>108.6019787529929</v>
+        <v>8.601978752992911</v>
       </c>
       <c r="E28" s="2">
-        <v>109.721890131482</v>
+        <v>9.721890131482029</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -2621,13 +2621,13 @@
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2">
-        <v>109.051601597595</v>
+        <v>9.051601597594949</v>
       </c>
       <c r="D29" s="2">
-        <v>107.611918043502</v>
+        <v>7.611918043502031</v>
       </c>
       <c r="E29" s="2">
-        <v>109.0300322919788</v>
+        <v>9.030032291978793</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -2636,13 +2636,13 @@
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2">
-        <v>106.5666906077168</v>
+        <v>6.566690607716823</v>
       </c>
       <c r="D30" s="2">
-        <v>106.8272018621244</v>
+        <v>6.827201862124387</v>
       </c>
       <c r="E30" s="2">
-        <v>108.1656551990757</v>
+        <v>8.165655199075662</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -2651,13 +2651,13 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2">
-        <v>105.6280249400627</v>
+        <v>5.62802494006268</v>
       </c>
       <c r="D31" s="2">
-        <v>106.8211268368127</v>
+        <v>6.821126836812724</v>
       </c>
       <c r="E31" s="2">
-        <v>108.1238878882766</v>
+        <v>8.123887888276622</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -2666,13 +2666,13 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D32" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E32" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -2681,13 +2681,13 @@
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D33" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E33" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -2696,13 +2696,13 @@
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D34" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E34" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -2711,13 +2711,13 @@
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D35" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E35" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -2726,13 +2726,13 @@
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D36" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E36" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -2741,13 +2741,13 @@
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D37" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E37" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -2756,13 +2756,13 @@
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2">
-        <v>141.7442130435599</v>
+        <v>41.7442130435599</v>
       </c>
       <c r="D38" s="2">
-        <v>140.1409664231686</v>
+        <v>40.14096642316861</v>
       </c>
       <c r="E38" s="2">
-        <v>143.461271155046</v>
+        <v>43.46127115504601</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -2771,13 +2771,13 @@
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2">
-        <v>117.9048074979183</v>
+        <v>17.90480749791825</v>
       </c>
       <c r="D39" s="2">
-        <v>114.6623810975685</v>
+        <v>14.66238109756853</v>
       </c>
       <c r="E39" s="2">
-        <v>118.4549776699289</v>
+        <v>18.45497766992889</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -2786,13 +2786,13 @@
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2">
-        <v>116.3179437560024</v>
+        <v>16.31794375600242</v>
       </c>
       <c r="D40" s="2">
-        <v>119.126401924712</v>
+        <v>19.12640192471202</v>
       </c>
       <c r="E40" s="2">
-        <v>122.4437430459023</v>
+        <v>22.44374304590231</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -2801,13 +2801,13 @@
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2">
-        <v>109.9752461808908</v>
+        <v>9.975246180890847</v>
       </c>
       <c r="D41" s="2">
-        <v>118.3491128670014</v>
+        <v>18.34911286700137</v>
       </c>
       <c r="E41" s="2">
-        <v>123.2056920173415</v>
+        <v>23.20569201734154</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -2816,13 +2816,13 @@
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2">
-        <v>118.1238187244034</v>
+        <v>18.12381872440342</v>
       </c>
       <c r="D42" s="2">
-        <v>115.2764931719222</v>
+        <v>15.2764931719222</v>
       </c>
       <c r="E42" s="2">
-        <v>119.3997172692221</v>
+        <v>19.39971726922204</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -2831,13 +2831,13 @@
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2">
-        <v>106.6086767449847</v>
+        <v>6.608676744984746</v>
       </c>
       <c r="D43" s="2">
-        <v>113.4838191485299</v>
+        <v>13.48381914852989</v>
       </c>
       <c r="E43" s="2">
-        <v>117.6148091351713</v>
+        <v>17.61480913517133</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2846,13 +2846,13 @@
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2">
-        <v>112.3202972412109</v>
+        <v>12.32029819488525</v>
       </c>
       <c r="D44" s="2">
-        <v>111.3030700683594</v>
+        <v>11.30306816101074</v>
       </c>
       <c r="E44" s="2">
-        <v>111.842399597168</v>
+        <v>11.84240341186523</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2861,13 +2861,13 @@
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2">
-        <v>114.3151168823242</v>
+        <v>14.31511688232422</v>
       </c>
       <c r="D45" s="2">
-        <v>107.5494537353516</v>
+        <v>7.549455165863037</v>
       </c>
       <c r="E45" s="2">
-        <v>109.3707275390625</v>
+        <v>9.370729446411133</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2891,13 +2891,13 @@
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2">
-        <v>122.9322967529297</v>
+        <v>22.93229484558105</v>
       </c>
       <c r="D47" s="2">
-        <v>120.7884521484375</v>
+        <v>20.78845024108887</v>
       </c>
       <c r="E47" s="2">
-        <v>123.14892578125</v>
+        <v>23.14892768859863</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2906,13 +2906,13 @@
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2">
-        <v>114.5723495483398</v>
+        <v>14.57234859466553</v>
       </c>
       <c r="D48" s="2">
-        <v>113.2040252685547</v>
+        <v>13.20402336120605</v>
       </c>
       <c r="E48" s="2">
-        <v>113.7573547363281</v>
+        <v>13.75735378265381</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2921,13 +2921,13 @@
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2">
-        <v>111.661750793457</v>
+        <v>11.66175270080566</v>
       </c>
       <c r="D49" s="2">
-        <v>108.5102615356445</v>
+        <v>8.510261535644531</v>
       </c>
       <c r="E49" s="2">
-        <v>109.7856826782227</v>
+        <v>9.785683631896973</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -2936,13 +2936,13 @@
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2">
-        <v>114.0274200439453</v>
+        <v>14.02741718292236</v>
       </c>
       <c r="D50" s="2">
-        <v>108.323356628418</v>
+        <v>8.323356628417969</v>
       </c>
       <c r="E50" s="2">
-        <v>111.0597229003906</v>
+        <v>11.05972194671631</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2951,13 +2951,13 @@
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2">
-        <v>108.2132720947266</v>
+        <v>8.213273048400879</v>
       </c>
       <c r="D51" s="2">
-        <v>108.2132720947266</v>
+        <v>8.213273048400879</v>
       </c>
       <c r="E51" s="2">
-        <v>108.2132720947266</v>
+        <v>8.213273048400879</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2966,13 +2966,13 @@
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2">
-        <v>114.3493194580078</v>
+        <v>14.3493185043335</v>
       </c>
       <c r="D52" s="2">
-        <v>116.0060729980469</v>
+        <v>16.00607490539551</v>
       </c>
       <c r="E52" s="2">
-        <v>119.6857528686523</v>
+        <v>19.68575477600098</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2981,13 +2981,13 @@
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2">
-        <v>113.9139022827148</v>
+        <v>13.91389846801758</v>
       </c>
       <c r="D53" s="2">
-        <v>110.5818710327148</v>
+        <v>10.58187007904053</v>
       </c>
       <c r="E53" s="2">
-        <v>111.8965606689453</v>
+        <v>11.89655685424805</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2996,13 +2996,13 @@
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2">
-        <v>111.4065017700195</v>
+        <v>11.4064998626709</v>
       </c>
       <c r="D54" s="2">
-        <v>108.8073043823242</v>
+        <v>8.807306289672852</v>
       </c>
       <c r="E54" s="2">
-        <v>110.0499496459961</v>
+        <v>10.04994773864746</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -3011,13 +3011,13 @@
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2">
-        <v>115.2005615234375</v>
+        <v>15.20055770874023</v>
       </c>
       <c r="D55" s="2">
-        <v>108.5818710327148</v>
+        <v>8.581871032714844</v>
       </c>
       <c r="E55" s="2">
-        <v>110.9671173095703</v>
+        <v>10.967116355896</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -3026,13 +3026,13 @@
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2">
-        <v>107.2044982910156</v>
+        <v>7.204496383666992</v>
       </c>
       <c r="D56" s="2">
-        <v>107.2044982910156</v>
+        <v>7.204496383666992</v>
       </c>
       <c r="E56" s="2">
-        <v>107.2044982910156</v>
+        <v>7.204496383666992</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -3041,13 +3041,13 @@
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2">
-        <v>113.8025817871094</v>
+        <v>13.80257987976074</v>
       </c>
       <c r="D57" s="2">
-        <v>115.0981063842773</v>
+        <v>15.09810543060303</v>
       </c>
       <c r="E57" s="2">
-        <v>118.8546524047852</v>
+        <v>18.85465240478516</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -3056,13 +3056,13 @@
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2">
-        <v>109.2754135131836</v>
+        <v>9.275417327880859</v>
       </c>
       <c r="D58" s="2">
-        <v>106.5745468139648</v>
+        <v>6.574543476104736</v>
       </c>
       <c r="E58" s="2">
-        <v>107.8064422607422</v>
+        <v>7.806442737579346</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -3071,13 +3071,13 @@
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2">
-        <v>111.4402313232422</v>
+        <v>11.44022941589355</v>
       </c>
       <c r="D59" s="2">
-        <v>108.4855270385742</v>
+        <v>8.485523223876953</v>
       </c>
       <c r="E59" s="2">
-        <v>110.432861328125</v>
+        <v>10.432861328125</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -3086,13 +3086,13 @@
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2">
-        <v>115.7983703613281</v>
+        <v>15.79836750030518</v>
       </c>
       <c r="D60" s="2">
-        <v>107.3515243530273</v>
+        <v>7.351525783538818</v>
       </c>
       <c r="E60" s="2">
-        <v>109.9095687866211</v>
+        <v>9.909566879272461</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -3101,13 +3101,13 @@
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2">
-        <v>106.3913955688477</v>
+        <v>6.391395092010498</v>
       </c>
       <c r="D61" s="2">
-        <v>106.3913955688477</v>
+        <v>6.391395092010498</v>
       </c>
       <c r="E61" s="2">
-        <v>106.3913955688477</v>
+        <v>6.391395092010498</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -3116,13 +3116,13 @@
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2">
-        <v>109.6991577148438</v>
+        <v>9.69915771484375</v>
       </c>
       <c r="D62" s="2">
-        <v>113.7160949707031</v>
+        <v>13.71609592437744</v>
       </c>
       <c r="E62" s="2">
-        <v>118.3788070678711</v>
+        <v>18.37880706787109</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -3131,13 +3131,13 @@
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2">
-        <v>103.6191787719727</v>
+        <v>3.619181156158447</v>
       </c>
       <c r="D63" s="2">
-        <v>100.9641647338867</v>
+        <v>0.9641610980033875</v>
       </c>
       <c r="E63" s="2">
-        <v>102.7881393432617</v>
+        <v>2.788138151168823</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -3146,13 +3146,13 @@
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2">
-        <v>108.0526351928711</v>
+        <v>8.052631378173828</v>
       </c>
       <c r="D64" s="2">
-        <v>107.7009811401367</v>
+        <v>7.700984477996826</v>
       </c>
       <c r="E64" s="2">
-        <v>109.5689926147461</v>
+        <v>9.56899356842041</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -3161,13 +3161,13 @@
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2">
-        <v>108.9937896728516</v>
+        <v>8.993790626525879</v>
       </c>
       <c r="D65" s="2">
-        <v>104.2914199829102</v>
+        <v>4.291417121887207</v>
       </c>
       <c r="E65" s="2">
-        <v>106.7485198974609</v>
+        <v>6.748517513275146</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -3176,13 +3176,13 @@
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2">
-        <v>105.8768997192383</v>
+        <v>5.876898288726807</v>
       </c>
       <c r="D66" s="2">
-        <v>105.8768997192383</v>
+        <v>5.876898288726807</v>
       </c>
       <c r="E66" s="2">
-        <v>105.8768997192383</v>
+        <v>5.876898288726807</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -3191,13 +3191,13 @@
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="2">
-        <v>105.8174667358398</v>
+        <v>5.817469596862793</v>
       </c>
       <c r="D67" s="2">
-        <v>114.2177886962891</v>
+        <v>14.21778964996338</v>
       </c>
       <c r="E67" s="2">
-        <v>117.9976348876953</v>
+        <v>17.99763298034668</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -3206,13 +3206,13 @@
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2">
-        <v>100.2247543334961</v>
+        <v>0.2247510552406311</v>
       </c>
       <c r="D68" s="2">
-        <v>99.93392944335938</v>
+        <v>-0.06607025116682053</v>
       </c>
       <c r="E68" s="2">
-        <v>101.6650161743164</v>
+        <v>1.6650151014328</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -3221,13 +3221,13 @@
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2">
-        <v>100.3374252319336</v>
+        <v>0.3374257683753967</v>
       </c>
       <c r="D69" s="2">
-        <v>105.1654663085938</v>
+        <v>5.165462970733643</v>
       </c>
       <c r="E69" s="2">
-        <v>106.7888488769531</v>
+        <v>6.7888503074646</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -3236,13 +3236,13 @@
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2">
-        <v>107.3705596923828</v>
+        <v>7.370556831359863</v>
       </c>
       <c r="D70" s="2">
-        <v>103.8991165161133</v>
+        <v>3.89911675453186</v>
       </c>
       <c r="E70" s="2">
-        <v>106.160888671875</v>
+        <v>6.160892486572266</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -3251,13 +3251,13 @@
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2">
-        <v>105.9054794311523</v>
+        <v>5.905477523803711</v>
       </c>
       <c r="D71" s="2">
-        <v>105.9054794311523</v>
+        <v>5.905477523803711</v>
       </c>
       <c r="E71" s="2">
-        <v>105.9054794311523</v>
+        <v>5.905477523803711</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -3266,13 +3266,13 @@
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2">
-        <v>104.9963073730469</v>
+        <v>4.996310710906982</v>
       </c>
       <c r="D72" s="2">
-        <v>114.1932830810547</v>
+        <v>14.19328212738037</v>
       </c>
       <c r="E72" s="2">
-        <v>117.6402359008789</v>
+        <v>17.64023590087891</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -3281,13 +3281,13 @@
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D73" s="2">
-        <v>104.9321594238281</v>
+        <v>4.93215799331665</v>
       </c>
       <c r="E73" s="2">
-        <v>106.5721893310547</v>
+        <v>6.57218599319458</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -3296,13 +3296,13 @@
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2">
-        <v>142.0969095486554</v>
+        <v>42.09690954865545</v>
       </c>
       <c r="D74" s="2">
-        <v>140.434925384026</v>
+        <v>40.43492538402597</v>
       </c>
       <c r="E74" s="2">
-        <v>143.6102090706754</v>
+        <v>43.61020907067537</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -3311,13 +3311,13 @@
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2">
-        <v>115.7775809164324</v>
+        <v>15.77758091643236</v>
       </c>
       <c r="D75" s="2">
-        <v>112.0281119280833</v>
+        <v>12.02811192808335</v>
       </c>
       <c r="E75" s="2">
-        <v>115.1755940471427</v>
+        <v>15.17559404714267</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -3326,13 +3326,13 @@
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2">
-        <v>114.695934706913</v>
+        <v>14.69593470691299</v>
       </c>
       <c r="D76" s="2">
-        <v>117.6768672379605</v>
+        <v>17.6768672379605</v>
       </c>
       <c r="E76" s="2">
-        <v>120.6150146970424</v>
+        <v>20.61501469704239</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -3341,13 +3341,13 @@
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2">
-        <v>109.3647425082543</v>
+        <v>9.364742508254336</v>
       </c>
       <c r="D77" s="2">
-        <v>116.9627812102758</v>
+        <v>16.96278121027581</v>
       </c>
       <c r="E77" s="2">
-        <v>121.2816057793425</v>
+        <v>21.28160577934251</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -3356,13 +3356,13 @@
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2">
-        <v>118.4482369946029</v>
+        <v>18.44823699460291</v>
       </c>
       <c r="D78" s="2">
-        <v>114.1711950798264</v>
+        <v>14.17119507982644</v>
       </c>
       <c r="E78" s="2">
-        <v>118.1768486927674</v>
+        <v>18.17684869276734</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -3371,13 +3371,13 @@
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="2">
-        <v>106.3477491799425</v>
+        <v>6.347749179942457</v>
       </c>
       <c r="D79" s="2">
-        <v>112.198235626183</v>
+        <v>12.19823562618298</v>
       </c>
       <c r="E79" s="2">
-        <v>116.2726895715698</v>
+        <v>16.27268957156985</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -3386,13 +3386,13 @@
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2">
-        <v>113.4294983956014</v>
+        <v>13.42949839560138</v>
       </c>
       <c r="D80" s="2">
-        <v>115.4259515180992</v>
+        <v>15.42595151809915</v>
       </c>
       <c r="E80" s="2">
-        <v>116.0967740022183</v>
+        <v>16.09677400221827</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -3401,13 +3401,13 @@
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2">
-        <v>106.0431602010029</v>
+        <v>6.043160201002927</v>
       </c>
       <c r="D81" s="2">
-        <v>101.8329248177095</v>
+        <v>1.832924817709523</v>
       </c>
       <c r="E81" s="2">
-        <v>103.2150119036671</v>
+        <v>3.215011903667143</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -3416,13 +3416,13 @@
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2">
-        <v>101.1114508032624</v>
+        <v>1.111450803262349</v>
       </c>
       <c r="D82" s="2">
-        <v>100.296204345676</v>
+        <v>0.2962043456760258</v>
       </c>
       <c r="E82" s="2">
-        <v>101.5641163979785</v>
+        <v>1.564116397978528</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -3431,13 +3431,13 @@
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2">
-        <v>110.0637886975012</v>
+        <v>10.06378869750115</v>
       </c>
       <c r="D83" s="2">
-        <v>106.0781541650525</v>
+        <v>6.078154165052493</v>
       </c>
       <c r="E83" s="2">
-        <v>108.1221885950163</v>
+        <v>8.122188595016343</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -3446,13 +3446,13 @@
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2">
-        <v>111.0307149693382</v>
+        <v>11.03071496933818</v>
       </c>
       <c r="D84" s="2">
-        <v>106.014930611548</v>
+        <v>6.014930611547988</v>
       </c>
       <c r="E84" s="2">
-        <v>107.8685820145409</v>
+        <v>7.868582014540919</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -3461,13 +3461,13 @@
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2">
-        <v>102.8545432052454</v>
+        <v>2.854543205245365</v>
       </c>
       <c r="D85" s="2">
-        <v>104.6840607719977</v>
+        <v>4.684060771997654</v>
       </c>
       <c r="E85" s="2">
-        <v>106.3092840368721</v>
+        <v>6.309284036872064</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -3476,13 +3476,13 @@
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="2">
-        <v>106.3806513824993</v>
+        <v>6.38065138249926</v>
       </c>
       <c r="D86" s="2">
-        <v>103.8284757887404</v>
+        <v>3.828475788740367</v>
       </c>
       <c r="E86" s="2">
-        <v>106.395944045844</v>
+        <v>6.395944045844014</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -3491,13 +3491,13 @@
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="2">
-        <v>112.7741561929101</v>
+        <v>12.77415619291012</v>
       </c>
       <c r="D87" s="2">
-        <v>112.0618444927675</v>
+        <v>12.06184449276755</v>
       </c>
       <c r="E87" s="2">
-        <v>115.2597085004402</v>
+        <v>15.25970850044019</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -3506,13 +3506,13 @@
       </c>
       <c r="B88" s="2"/>
       <c r="C88" s="2">
-        <v>113.4019669460993</v>
+        <v>13.40196694609931</v>
       </c>
       <c r="D88" s="2">
-        <v>116.8535346712863</v>
+        <v>16.85353467128634</v>
       </c>
       <c r="E88" s="2">
-        <v>118.9172571345435</v>
+        <v>18.91725713454354</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -3521,13 +3521,13 @@
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="2">
-        <v>114.3734758810617</v>
+        <v>14.37347588106172</v>
       </c>
       <c r="D89" s="2">
-        <v>104.3268044103817</v>
+        <v>4.326804410381691</v>
       </c>
       <c r="E89" s="2">
-        <v>106.117051103353</v>
+        <v>6.117051103352965</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -3536,13 +3536,13 @@
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="2">
-        <v>116.6600919190665</v>
+        <v>16.66009191906645</v>
       </c>
       <c r="D90" s="2">
-        <v>102.1215202231729</v>
+        <v>2.121520223172912</v>
       </c>
       <c r="E90" s="2">
-        <v>103.718287976195</v>
+        <v>3.71828797619504</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -3551,13 +3551,13 @@
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="2">
-        <v>107.8550008014949</v>
+        <v>7.855000801494898</v>
       </c>
       <c r="D91" s="2">
-        <v>104.3352478258511</v>
+        <v>4.335247825851105</v>
       </c>
       <c r="E91" s="2">
-        <v>106.5730290242286</v>
+        <v>6.57302902422855</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -3566,13 +3566,13 @@
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="2">
-        <v>141.2462908011869</v>
+        <v>41.24629080118694</v>
       </c>
       <c r="D92" s="2">
-        <v>139.4658753709199</v>
+        <v>39.4658753709199</v>
       </c>
       <c r="E92" s="2">
-        <v>142.1364985163205</v>
+        <v>42.13649851632051</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -3581,13 +3581,13 @@
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="2">
-        <v>115.9663865546219</v>
+        <v>15.96638655462187</v>
       </c>
       <c r="D93" s="2">
-        <v>112.3404255319149</v>
+        <v>12.3404255319149</v>
       </c>
       <c r="E93" s="2">
-        <v>115.2400835073069</v>
+        <v>15.24008350730688</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -3596,13 +3596,13 @@
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="2">
-        <v>114.3115942028985</v>
+        <v>14.31159420289855</v>
       </c>
       <c r="D94" s="2">
-        <v>117.8030303030303</v>
+        <v>17.8030303030303</v>
       </c>
       <c r="E94" s="2">
-        <v>120.8333333333333</v>
+        <v>20.83333333333333</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -3611,13 +3611,13 @@
       </c>
       <c r="B95" s="2"/>
       <c r="C95" s="2">
-        <v>109.6671949286846</v>
+        <v>9.667194928684628</v>
       </c>
       <c r="D95" s="2">
-        <v>116.5594855305467</v>
+        <v>16.55948553054664</v>
       </c>
       <c r="E95" s="2">
-        <v>121.4392803598201</v>
+        <v>21.43928035982008</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -3626,13 +3626,13 @@
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2">
-        <v>118.3526011560694</v>
+        <v>18.35260115606937</v>
       </c>
       <c r="D96" s="2">
-        <v>114.2068965517241</v>
+        <v>14.20689655172409</v>
       </c>
       <c r="E96" s="2">
-        <v>118.3950617283951</v>
+        <v>18.39506172839507</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -3641,13 +3641,13 @@
       </c>
       <c r="B97" s="2"/>
       <c r="C97" s="2">
-        <v>106.7155067155067</v>
+        <v>6.715506715506716</v>
       </c>
       <c r="D97" s="2">
-        <v>112.56038647343</v>
+        <v>12.56038647343</v>
       </c>
       <c r="E97" s="2">
-        <v>116.162669447341</v>
+        <v>16.16266944734096</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -3656,13 +3656,13 @@
       </c>
       <c r="B98" s="2"/>
       <c r="C98" s="2">
-        <v>127.33147663382</v>
+        <v>27.33147663382004</v>
       </c>
       <c r="D98" s="2">
-        <v>130.2807008982568</v>
+        <v>30.28070089825683</v>
       </c>
       <c r="E98" s="2">
-        <v>133.7545182980177</v>
+        <v>33.75451829801769</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -3671,13 +3671,13 @@
       </c>
       <c r="B99" s="2"/>
       <c r="C99" s="2">
-        <v>116.1886120996441</v>
+        <v>16.18861209964412</v>
       </c>
       <c r="D99" s="2">
-        <v>115.5187405855613</v>
+        <v>15.51874058556133</v>
       </c>
       <c r="E99" s="2">
-        <v>119.8312863051076</v>
+        <v>19.83128630510755</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -3686,13 +3686,13 @@
       </c>
       <c r="B100" s="2"/>
       <c r="C100" s="2">
-        <v>114.8139771037869</v>
+        <v>14.81397710378691</v>
       </c>
       <c r="D100" s="2">
-        <v>112.3810692878517</v>
+        <v>12.38106928785171</v>
       </c>
       <c r="E100" s="2">
-        <v>115.5289512314468</v>
+        <v>15.52895123144674</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -3701,13 +3701,13 @@
       </c>
       <c r="B101" s="2"/>
       <c r="C101" s="2">
-        <v>109.1212424047789</v>
+        <v>9.121242404778847</v>
       </c>
       <c r="D101" s="2">
-        <v>116.5549306398528</v>
+        <v>16.55493063985276</v>
       </c>
       <c r="E101" s="2">
-        <v>120.5503820371929</v>
+        <v>20.55038203719288</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -3716,13 +3716,13 @@
       </c>
       <c r="B102" s="2"/>
       <c r="C102" s="2">
-        <v>121.5786385638688</v>
+        <v>21.57863856386881</v>
       </c>
       <c r="D102" s="2">
-        <v>118.6196067891554</v>
+        <v>18.61960678915535</v>
       </c>
       <c r="E102" s="2">
-        <v>121.6434702631632</v>
+        <v>21.64347026316323</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -3731,13 +3731,13 @@
       </c>
       <c r="B103" s="2"/>
       <c r="C103" s="2">
-        <v>106.8000600146324</v>
+        <v>6.800060014632427</v>
       </c>
       <c r="D103" s="2">
-        <v>114.7075659012718</v>
+        <v>14.70756590127178</v>
       </c>
       <c r="E103" s="2">
-        <v>118.2125683242491</v>
+        <v>18.2125683242491</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -3746,13 +3746,13 @@
       </c>
       <c r="B104" s="2"/>
       <c r="C104" s="2">
-        <v>123.1392129562949</v>
+        <v>23.13921295629492</v>
       </c>
       <c r="D104" s="2">
-        <v>125.2980619968953</v>
+        <v>25.29806199689536</v>
       </c>
       <c r="E104" s="2">
-        <v>126.0230127866596</v>
+        <v>26.02301278665965</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -3761,13 +3761,13 @@
       </c>
       <c r="B105" s="2"/>
       <c r="C105" s="2">
-        <v>114.3269305746887</v>
+        <v>14.32693057468874</v>
       </c>
       <c r="D105" s="2">
-        <v>109.8013921706367</v>
+        <v>9.80139217063669</v>
       </c>
       <c r="E105" s="2">
-        <v>111.2625082541779</v>
+        <v>11.26250825417788</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -3776,13 +3776,13 @@
       </c>
       <c r="B106" s="2"/>
       <c r="C106" s="2">
-        <v>100.9969307718541</v>
+        <v>0.9969307718540494</v>
       </c>
       <c r="D106" s="2">
-        <v>100.151217299259</v>
+        <v>0.1512172992590352</v>
       </c>
       <c r="E106" s="2">
-        <v>101.4380770854971</v>
+        <v>1.438077085497086</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -3791,13 +3791,13 @@
       </c>
       <c r="B107" s="2"/>
       <c r="C107" s="2">
-        <v>99.18849257712696</v>
+        <v>-0.811507422873033</v>
       </c>
       <c r="D107" s="2">
-        <v>95.7119130303488</v>
+        <v>-4.288086969651203</v>
       </c>
       <c r="E107" s="2">
-        <v>97.55729828864612</v>
+        <v>-2.442701711353878</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -3806,13 +3806,13 @@
       </c>
       <c r="B108" s="2"/>
       <c r="C108" s="2">
-        <v>100.6740349045685</v>
+        <v>0.6740349045684546</v>
       </c>
       <c r="D108" s="2">
-        <v>96.06708167995436</v>
+        <v>-3.932918320045643</v>
       </c>
       <c r="E108" s="2">
-        <v>97.73948746338201</v>
+        <v>-2.260512536617997</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -3821,13 +3821,13 @@
       </c>
       <c r="B109" s="2"/>
       <c r="C109" s="2">
-        <v>101.2443642921551</v>
+        <v>1.244364292155111</v>
       </c>
       <c r="D109" s="2">
-        <v>102.992446252179</v>
+        <v>2.992446252178973</v>
       </c>
       <c r="E109" s="2">
-        <v>104.590187147476</v>
+        <v>4.590187147475965</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -4585,10 +4585,10 @@
         <v>162</v>
       </c>
       <c r="B160" s="2"/>
-      <c r="C160" s="2">
+      <c r="C160" s="3">
         <v>-522.1999999999989</v>
       </c>
-      <c r="D160" s="2">
+      <c r="D160" s="3">
         <v>-266</v>
       </c>
       <c r="E160" s="2">
@@ -5080,7 +5080,7 @@
         <v>195</v>
       </c>
       <c r="B193" s="2"/>
-      <c r="C193" s="2">
+      <c r="C193" s="3">
         <v>-475</v>
       </c>
       <c r="D193" s="3">
@@ -5350,13 +5350,13 @@
         <v>213</v>
       </c>
       <c r="B211" s="2"/>
-      <c r="C211" s="2">
+      <c r="C211" s="3">
         <v>-229.4000000000015</v>
       </c>
-      <c r="D211" s="2">
+      <c r="D211" s="3">
         <v>-164.6000000000004</v>
       </c>
-      <c r="E211" s="2">
+      <c r="E211" s="3">
         <v>-174.2000000000007</v>
       </c>
     </row>
@@ -5980,13 +5980,13 @@
         <v>255</v>
       </c>
       <c r="B253" s="2"/>
-      <c r="C253" s="2">
+      <c r="C253" s="3">
         <v>-4845.600000000006</v>
       </c>
-      <c r="D253" s="2">
+      <c r="D253" s="3">
         <v>-4424.599999999999</v>
       </c>
-      <c r="E253" s="2">
+      <c r="E253" s="3">
         <v>-4758.200000000004</v>
       </c>
     </row>
@@ -6025,13 +6025,13 @@
         <v>258</v>
       </c>
       <c r="B256" s="2"/>
-      <c r="C256" s="2">
+      <c r="C256" s="3">
         <v>-5741.800000000003</v>
       </c>
-      <c r="D256" s="2">
+      <c r="D256" s="3">
         <v>-5307.599999999999</v>
       </c>
-      <c r="E256" s="2">
+      <c r="E256" s="3">
         <v>-5731.199999999997</v>
       </c>
     </row>
@@ -7375,13 +7375,13 @@
         <v>348</v>
       </c>
       <c r="B346" s="2"/>
-      <c r="C346" s="2">
+      <c r="C346" s="3">
         <v>-270</v>
       </c>
-      <c r="D346" s="2">
+      <c r="D346" s="3">
         <v>-444.3999999999996</v>
       </c>
-      <c r="E346" s="2">
+      <c r="E346" s="3">
         <v>-441.5999999999999</v>
       </c>
     </row>
@@ -7423,10 +7423,10 @@
       <c r="C349" s="2">
         <v>-83.19999999999982</v>
       </c>
-      <c r="D349" s="2">
+      <c r="D349" s="3">
         <v>-611.2000000000003</v>
       </c>
-      <c r="E349" s="2">
+      <c r="E349" s="3">
         <v>-566.8000000000002</v>
       </c>
     </row>
@@ -7645,13 +7645,13 @@
         <v>366</v>
       </c>
       <c r="B364" s="2"/>
-      <c r="C364" s="2">
+      <c r="C364" s="3">
         <v>-111.4000000000001</v>
       </c>
-      <c r="D364" s="2">
+      <c r="D364" s="3">
         <v>-111.4000000000001</v>
       </c>
-      <c r="E364" s="2">
+      <c r="E364" s="3">
         <v>-111.4000000000001</v>
       </c>
     </row>
@@ -7690,13 +7690,13 @@
         <v>369</v>
       </c>
       <c r="B367" s="2"/>
-      <c r="C367" s="2">
+      <c r="C367" s="3">
         <v>-611</v>
       </c>
-      <c r="D367" s="2">
+      <c r="D367" s="3">
         <v>-626</v>
       </c>
-      <c r="E367" s="2">
+      <c r="E367" s="3">
         <v>-640</v>
       </c>
     </row>
@@ -7735,13 +7735,13 @@
         <v>372</v>
       </c>
       <c r="B370" s="2"/>
-      <c r="C370" s="2">
+      <c r="C370" s="3">
         <v>-613.5999999999999</v>
       </c>
-      <c r="D370" s="2">
+      <c r="D370" s="3">
         <v>-574.5999999999999</v>
       </c>
-      <c r="E370" s="2">
+      <c r="E370" s="3">
         <v>-596.5999999999999</v>
       </c>
     </row>
@@ -7780,13 +7780,13 @@
         <v>375</v>
       </c>
       <c r="B373" s="2"/>
-      <c r="C373" s="2">
+      <c r="C373" s="3">
         <v>-591.4000000000001</v>
       </c>
-      <c r="D373" s="2">
+      <c r="D373" s="3">
         <v>-495.4000000000001</v>
       </c>
-      <c r="E373" s="2">
+      <c r="E373" s="3">
         <v>-537.4000000000001</v>
       </c>
     </row>
@@ -7825,13 +7825,13 @@
         <v>378</v>
       </c>
       <c r="B376" s="2"/>
-      <c r="C376" s="2">
+      <c r="C376" s="3">
         <v>-585</v>
       </c>
-      <c r="D376" s="2">
+      <c r="D376" s="3">
         <v>-427</v>
       </c>
-      <c r="E376" s="2">
+      <c r="E376" s="3">
         <v>-513</v>
       </c>
     </row>
@@ -7870,13 +7870,13 @@
         <v>381</v>
       </c>
       <c r="B379" s="2"/>
-      <c r="C379" s="2">
+      <c r="C379" s="3">
         <v>-1426</v>
       </c>
-      <c r="D379" s="2">
+      <c r="D379" s="3">
         <v>-1275</v>
       </c>
-      <c r="E379" s="2">
+      <c r="E379" s="3">
         <v>-1354</v>
       </c>
     </row>
@@ -7915,13 +7915,13 @@
         <v>384</v>
       </c>
       <c r="B382" s="2"/>
-      <c r="C382" s="2">
+      <c r="C382" s="3">
         <v>-1381.6</v>
       </c>
-      <c r="D382" s="2">
+      <c r="D382" s="3">
         <v>-1238.6</v>
       </c>
-      <c r="E382" s="2">
+      <c r="E382" s="3">
         <v>-1315.6</v>
       </c>
     </row>
@@ -8413,10 +8413,10 @@
       <c r="C415" s="2">
         <v>18.79999999999927</v>
       </c>
-      <c r="D415" s="2">
+      <c r="D415" s="3">
         <v>-1028.4</v>
       </c>
-      <c r="E415" s="2">
+      <c r="E415" s="3">
         <v>-612.3999999999996</v>
       </c>
     </row>
@@ -8458,7 +8458,7 @@
       <c r="C418" s="3">
         <v>248.2000000000007</v>
       </c>
-      <c r="D418" s="2">
+      <c r="D418" s="3">
         <v>-991.2000000000007</v>
       </c>
       <c r="E418" s="2">
@@ -8500,10 +8500,10 @@
         <v>423</v>
       </c>
       <c r="B421" s="2"/>
-      <c r="C421" s="2">
+      <c r="C421" s="3">
         <v>-745.5999999999985</v>
       </c>
-      <c r="D421" s="2">
+      <c r="D421" s="3">
         <v>-1591.799999999999</v>
       </c>
       <c r="E421" s="3">
@@ -8548,7 +8548,7 @@
       <c r="C424" s="3">
         <v>527.5999999999985</v>
       </c>
-      <c r="D424" s="2">
+      <c r="D424" s="3">
         <v>-1330.199999999999</v>
       </c>
       <c r="E424" s="3">
@@ -8635,13 +8635,13 @@
         <v>432</v>
       </c>
       <c r="B430" s="2"/>
-      <c r="C430" s="2">
+      <c r="C430" s="3">
         <v>-925.8</v>
       </c>
-      <c r="D430" s="2">
+      <c r="D430" s="3">
         <v>-866.5999999999999</v>
       </c>
-      <c r="E430" s="2">
+      <c r="E430" s="3">
         <v>-880.4000000000001</v>
       </c>
     </row>
@@ -8680,13 +8680,13 @@
         <v>435</v>
       </c>
       <c r="B433" s="2"/>
-      <c r="C433" s="2">
+      <c r="C433" s="3">
         <v>-947.5999999999999</v>
       </c>
-      <c r="D433" s="2">
+      <c r="D433" s="3">
         <v>-889.4000000000001</v>
       </c>
-      <c r="E433" s="2">
+      <c r="E433" s="3">
         <v>-908</v>
       </c>
     </row>
@@ -8725,13 +8725,13 @@
         <v>438</v>
       </c>
       <c r="B436" s="2"/>
-      <c r="C436" s="2">
+      <c r="C436" s="3">
         <v>-1002.8</v>
       </c>
-      <c r="D436" s="2">
+      <c r="D436" s="3">
         <v>-928.8</v>
       </c>
-      <c r="E436" s="2">
+      <c r="E436" s="3">
         <v>-955.4000000000001</v>
       </c>
     </row>
@@ -8770,13 +8770,13 @@
         <v>441</v>
       </c>
       <c r="B439" s="2"/>
-      <c r="C439" s="2">
+      <c r="C439" s="3">
         <v>-1017</v>
       </c>
-      <c r="D439" s="2">
+      <c r="D439" s="3">
         <v>-914.8</v>
       </c>
-      <c r="E439" s="2">
+      <c r="E439" s="3">
         <v>-941.2</v>
       </c>
     </row>
@@ -8815,13 +8815,13 @@
         <v>444</v>
       </c>
       <c r="B442" s="2"/>
-      <c r="C442" s="2">
+      <c r="C442" s="3">
         <v>-885</v>
       </c>
-      <c r="D442" s="2">
+      <c r="D442" s="3">
         <v>-810</v>
       </c>
-      <c r="E442" s="2">
+      <c r="E442" s="3">
         <v>-791.4000000000001</v>
       </c>
     </row>
@@ -8860,13 +8860,13 @@
         <v>447</v>
       </c>
       <c r="B445" s="2"/>
-      <c r="C445" s="2">
+      <c r="C445" s="3">
         <v>-772.2</v>
       </c>
-      <c r="D445" s="2">
+      <c r="D445" s="3">
         <v>-704.5999999999999</v>
       </c>
-      <c r="E445" s="2">
+      <c r="E445" s="3">
         <v>-642.6000000000001</v>
       </c>
     </row>
@@ -9130,10 +9130,10 @@
         <v>465</v>
       </c>
       <c r="B463" s="2"/>
-      <c r="C463" s="2">
+      <c r="C463" s="3">
         <v>-217</v>
       </c>
-      <c r="D463" s="2">
+      <c r="D463" s="3">
         <v>-202.3999999999996</v>
       </c>
       <c r="E463" s="2">
@@ -9175,7 +9175,7 @@
         <v>468</v>
       </c>
       <c r="B466" s="2"/>
-      <c r="C466" s="2">
+      <c r="C466" s="3">
         <v>-144</v>
       </c>
       <c r="D466" s="2">
@@ -9445,13 +9445,13 @@
         <v>486</v>
       </c>
       <c r="B484" s="2"/>
-      <c r="C484" s="2">
+      <c r="C484" s="3">
         <v>-1193</v>
       </c>
       <c r="D484" s="3">
         <v>134.3999999999996</v>
       </c>
-      <c r="E484" s="2">
+      <c r="E484" s="3">
         <v>-219.1999999999998</v>
       </c>
     </row>
@@ -9490,13 +9490,13 @@
         <v>489</v>
       </c>
       <c r="B487" s="2"/>
-      <c r="C487" s="2">
+      <c r="C487" s="3">
         <v>-1637.799999999999</v>
       </c>
       <c r="D487" s="2">
         <v>-65.19999999999982</v>
       </c>
-      <c r="E487" s="2">
+      <c r="E487" s="3">
         <v>-417.3999999999996</v>
       </c>
     </row>
@@ -9673,7 +9673,7 @@
       <c r="C499" s="3">
         <v>678.1999999999971</v>
       </c>
-      <c r="D499" s="2">
+      <c r="D499" s="3">
         <v>-444.1999999999971</v>
       </c>
       <c r="E499" s="3">
@@ -9760,13 +9760,13 @@
         <v>507</v>
       </c>
       <c r="B505" s="2"/>
-      <c r="C505" s="2">
+      <c r="C505" s="3">
         <v>-8943.399999999994</v>
       </c>
       <c r="D505" s="3">
         <v>9490</v>
       </c>
-      <c r="E505" s="2">
+      <c r="E505" s="3">
         <v>-2956.600000000006</v>
       </c>
     </row>
@@ -9805,10 +9805,10 @@
         <v>510</v>
       </c>
       <c r="B508" s="2"/>
-      <c r="C508" s="2">
+      <c r="C508" s="3">
         <v>-6563.600000000006</v>
       </c>
-      <c r="D508" s="2">
+      <c r="D508" s="3">
         <v>-505.6000000000058</v>
       </c>
       <c r="E508" s="3">
@@ -10075,13 +10075,13 @@
         <v>528</v>
       </c>
       <c r="B526" s="2"/>
-      <c r="C526" s="2">
+      <c r="C526" s="3">
         <v>-875</v>
       </c>
       <c r="D526" s="3">
         <v>508.6000000000004</v>
       </c>
-      <c r="E526" s="2">
+      <c r="E526" s="3">
         <v>-547.8000000000002</v>
       </c>
     </row>
@@ -10120,13 +10120,13 @@
         <v>531</v>
       </c>
       <c r="B529" s="2"/>
-      <c r="C529" s="2">
+      <c r="C529" s="3">
         <v>-797.2000000000007</v>
       </c>
       <c r="D529" s="3">
         <v>479.8000000000002</v>
       </c>
-      <c r="E529" s="2">
+      <c r="E529" s="3">
         <v>-502.5999999999995</v>
       </c>
     </row>
@@ -10390,10 +10390,10 @@
         <v>549</v>
       </c>
       <c r="B547" s="2"/>
-      <c r="C547" s="2">
+      <c r="C547" s="3">
         <v>-2225.600000000006</v>
       </c>
-      <c r="D547" s="2">
+      <c r="D547" s="3">
         <v>-322.3999999999942</v>
       </c>
       <c r="E547" s="3">
@@ -10435,13 +10435,13 @@
         <v>552</v>
       </c>
       <c r="B550" s="2"/>
-      <c r="C550" s="2">
+      <c r="C550" s="3">
         <v>-5028.199999999997</v>
       </c>
-      <c r="D550" s="2">
+      <c r="D550" s="3">
         <v>-2354.600000000006</v>
       </c>
-      <c r="E550" s="2">
+      <c r="E550" s="3">
         <v>-1521</v>
       </c>
     </row>
@@ -10525,13 +10525,13 @@
         <v>558</v>
       </c>
       <c r="B556" s="2"/>
-      <c r="C556" s="2">
+      <c r="C556" s="3">
         <v>-517.2000000000003</v>
       </c>
-      <c r="D556" s="2">
+      <c r="D556" s="3">
         <v>-650.4000000000001</v>
       </c>
-      <c r="E556" s="2">
+      <c r="E556" s="3">
         <v>-642.1999999999998</v>
       </c>
     </row>
@@ -10570,13 +10570,13 @@
         <v>561</v>
       </c>
       <c r="B559" s="2"/>
-      <c r="C559" s="2">
+      <c r="C559" s="3">
         <v>-399.1999999999998</v>
       </c>
-      <c r="D559" s="2">
+      <c r="D559" s="3">
         <v>-856.4000000000001</v>
       </c>
-      <c r="E559" s="2">
+      <c r="E559" s="3">
         <v>-788.8000000000002</v>
       </c>
     </row>
@@ -10618,10 +10618,10 @@
       <c r="C562" s="2">
         <v>-89.59999999999991</v>
       </c>
-      <c r="D562" s="2">
+      <c r="D562" s="3">
         <v>-964</v>
       </c>
-      <c r="E562" s="2">
+      <c r="E562" s="3">
         <v>-535.7999999999997</v>
       </c>
     </row>
@@ -10663,10 +10663,10 @@
       <c r="C565" s="2">
         <v>-30</v>
       </c>
-      <c r="D565" s="2">
+      <c r="D565" s="3">
         <v>-890.8000000000002</v>
       </c>
-      <c r="E565" s="2">
+      <c r="E565" s="3">
         <v>-197.7999999999997</v>
       </c>
     </row>
@@ -10708,7 +10708,7 @@
       <c r="C568" s="3">
         <v>249.6000000000004</v>
       </c>
-      <c r="D568" s="2">
+      <c r="D568" s="3">
         <v>-1092.4</v>
       </c>
       <c r="E568" s="3">
@@ -10753,7 +10753,7 @@
       <c r="C571" s="3">
         <v>248.2000000000007</v>
       </c>
-      <c r="D571" s="2">
+      <c r="D571" s="3">
         <v>-1006.2</v>
       </c>
       <c r="E571" s="3">

</xml_diff>